<commit_message>
Add templates nivel 0
</commit_message>
<xml_diff>
--- a/Data/Template - Nivel 0.xlsx
+++ b/Data/Template - Nivel 0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/tania_a_favila_perez_mx_ey_com/Documents/Documents/UiPath/Forensics v2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Forensics\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="6_{E714DA49-FBBC-464F-A27F-39342C0D6A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{972D362A-D44F-4DD2-A7A5-959E7FA6A8DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12174954-7020-4AAF-B6B3-8AECF17EBF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{59751C8B-1377-4162-816A-50DBE466B7D8}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{59751C8B-1377-4162-816A-50DBE466B7D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>NombreLegal</t>
   </si>
@@ -132,37 +132,7 @@
     <t>Puesto10</t>
   </si>
   <si>
-    <t>Ana Flavia Dos Santos  Pacheco Vizzotto</t>
-  </si>
-  <si>
-    <t>Claudia Iveth Pompa Ruiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GoGlobal Geo Limited   </t>
-  </si>
-  <si>
-    <t>GoGlobal Geo Mexico S de RL de CV</t>
-  </si>
-  <si>
-    <t>GoGlobal Geo Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GoGlobal KK  </t>
-  </si>
-  <si>
-    <t>Gerente General y Director</t>
-  </si>
-  <si>
-    <t>Gerente Senior</t>
-  </si>
-  <si>
-    <t>Carlos de Jesus Cano Reyes</t>
-  </si>
-  <si>
-    <t>Apoderado</t>
-  </si>
-  <si>
-    <t>Erick Ariel Sotelo Macias</t>
+    <t>Maria Teresa del Socorro Cazola Bravo</t>
   </si>
 </sst>
 </file>
@@ -521,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46D36C2-0EA7-4E97-A91A-C7C0BCB5306F}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
@@ -536,7 +506,7 @@
     <col min="12" max="12" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,57 +604,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.999</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>34</v>
-      </c>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AH2" t="s">
         <v>32</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nivel 0/Add Fecha and Pais
</commit_message>
<xml_diff>
--- a/Data/Template - Nivel 0.xlsx
+++ b/Data/Template - Nivel 0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Forensics\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8414B460-30CB-47E1-8C56-5946588DEA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA623836-CE05-4922-B8BE-8B0195C75B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4410" yWindow="1695" windowWidth="21600" windowHeight="11505" xr2:uid="{59751C8B-1377-4162-816A-50DBE466B7D8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>NombreLegal</t>
   </si>
@@ -141,37 +141,52 @@
     <t>Primarios4</t>
   </si>
   <si>
-    <t>Garay Componentes Tubulares SA de CV</t>
-  </si>
-  <si>
-    <t>Garay Componentes Tubulares</t>
-  </si>
-  <si>
-    <t>GCT150821KD7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garay Internationla XXI SLU  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hijos de Juan Garay SA  </t>
-  </si>
-  <si>
-    <t>Leopoldo Matos Castaño</t>
-  </si>
-  <si>
-    <t>Administrador Único</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedro Javier Mendoza </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director de Planta </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meztli  Aurora  Martinez </t>
-  </si>
-  <si>
-    <t>Directora de Finanzas</t>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>19 octubre 2023</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>Swiss Steel Mexico SA de CV</t>
+  </si>
+  <si>
+    <t>Swiss Steel Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	SSB9512118M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swiss Steel International  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiery Jean Denis Cremailh </t>
+  </si>
+  <si>
+    <t>Presidente</t>
+  </si>
+  <si>
+    <t>Sara Toriz Escamilla</t>
+  </si>
+  <si>
+    <t>Secretario</t>
+  </si>
+  <si>
+    <t>Fermin Huerta Rodriguez</t>
+  </si>
+  <si>
+    <t>Comisario</t>
+  </si>
+  <si>
+    <t>Jose Antonio Flores Muñoz</t>
+  </si>
+  <si>
+    <t>Apoderado</t>
   </si>
 </sst>
 </file>
@@ -530,19 +545,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46D36C2-0EA7-4E97-A91A-C7C0BCB5306F}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -551,8 +564,8 @@
     <col min="11" max="11" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
@@ -569,161 +582,172 @@
     <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.999</v>
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="N2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AG2" t="s">
         <v>43</v>
-      </c>
-      <c r="R2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>